<commit_message>
update test data with sub ses pref
</commit_message>
<xml_diff>
--- a/tests/test_data/subject_data.xlsx
+++ b/tests/test_data/subject_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzliem/Dropbox/Workspace/dynagefw/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC8250E-690A-D840-B029-7A8D6C353B6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF079D50-45FB-4F46-AA1A-03C5D813C1A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16060" xr2:uid="{350B5982-992D-C64F-912C-B80C52726BF8}"/>
   </bookViews>
@@ -33,12 +33,6 @@
     <t>hair</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
@@ -52,6 +46,12 @@
   </si>
   <si>
     <t>blond</t>
+  </si>
+  <si>
+    <t>sub-s1</t>
+  </si>
+  <si>
+    <t>sub-s2</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -416,7 +416,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -424,24 +424,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>